<commit_message>
Confirmed that lowering T1L bound to 10 doesn't really change much
</commit_message>
<xml_diff>
--- a/LacTissue0222final_0412_updated.xlsx
+++ b/LacTissue0222final_0412_updated.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B630C58E-8371-4B77-8FE6-144447C8170D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E50F786-CCF1-4FF1-9312-60D2CEF0C3B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CA065B6-2B6A-4D01-BE68-6D40353B42D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -143,13 +144,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2186,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965EB12B-5679-47D6-8B59-2B80512DA255}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,10 +2227,10 @@
       <c r="H1" s="2">
         <v>0.99710470753466751</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="6">
         <v>5.8059472924239228E-2</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="6">
         <v>9.8544279420448674E-2</v>
       </c>
     </row>
@@ -2254,10 +2259,10 @@
       <c r="H2" s="3">
         <v>0.98383286985676055</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="7">
         <v>0.18152987855890426</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="7">
         <v>0.17869625169151973</v>
       </c>
     </row>
@@ -2286,10 +2291,10 @@
       <c r="H3" s="1">
         <v>0.96991388828412761</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="8">
         <v>9.5480835703879982E-2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="8">
         <v>0.25588656191366183</v>
       </c>
     </row>
@@ -2318,10 +2323,10 @@
       <c r="H4" s="1">
         <v>0.98978317472692023</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="8">
         <v>8.4606566404595684E-2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="8">
         <v>0.14836296163036</v>
       </c>
     </row>
@@ -2350,10 +2355,10 @@
       <c r="H5" s="1">
         <v>0.71060677292707231</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="8">
         <v>7.2125770024450864E-2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="8">
         <v>0.92655284129541671</v>
       </c>
       <c r="L5" s="1">
@@ -2404,10 +2409,10 @@
       <c r="H6" s="3">
         <v>0.99636198364293327</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="7">
         <v>6.2826595309449007E-2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="7">
         <v>9.0333970116593318E-2</v>
       </c>
       <c r="L6">
@@ -2456,10 +2461,10 @@
       <c r="H7" s="3">
         <v>0.96604532309012181</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="7">
         <v>0.12417091868912668</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="7">
         <v>0.27077335890718474</v>
       </c>
     </row>
@@ -2488,10 +2493,10 @@
       <c r="H8" s="2">
         <v>0.99203900822419144</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="6">
         <v>9.0594478512034893E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="6">
         <v>0.13610334184766176</v>
       </c>
     </row>
@@ -2520,10 +2525,10 @@
       <c r="H9" s="2">
         <v>0.98739267714383039</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="6">
         <v>9.8942640570406248E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="6">
         <v>0.15737580320906272</v>
       </c>
     </row>
@@ -2552,10 +2557,10 @@
       <c r="H10" s="3">
         <v>0.97201111126300721</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="7">
         <v>0.13021444685847422</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="7">
         <v>0.24211458591708007</v>
       </c>
     </row>
@@ -2584,10 +2589,10 @@
       <c r="H11" s="2">
         <v>0.99230699527864108</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="6">
         <v>8.3898040655969397E-2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="6">
         <v>0.12480884052850011</v>
       </c>
       <c r="P11" t="s">
@@ -2622,10 +2627,10 @@
       <c r="H12" s="2">
         <v>0.99460822572338958</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="6">
         <v>0.10664313840326221</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="6">
         <v>0.10320484896225612</v>
       </c>
       <c r="P12">
@@ -2660,10 +2665,10 @@
       <c r="H13" s="4">
         <v>0.99777223030995432</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="9">
         <v>9.1508833243368184E-2</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="9">
         <v>7.0623847783424717E-2</v>
       </c>
       <c r="M13" s="2">
@@ -2700,10 +2705,10 @@
       <c r="H14" s="5">
         <v>0.45096404612170349</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="9">
         <v>0.12510825377174215</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="9">
         <v>1.3349999531484675</v>
       </c>
       <c r="M14" s="2">
@@ -2740,10 +2745,10 @@
       <c r="H15" s="4">
         <v>0.89266589363988524</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="9">
         <v>8.117543901175181E-2</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="9">
         <v>0.5430912460826407</v>
       </c>
       <c r="M15" s="2">
@@ -2786,10 +2791,10 @@
       <c r="H16" s="4">
         <v>0.97719118228161661</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="9">
         <v>6.0434518608142064E-2</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="9">
         <v>0.23983072412696493</v>
       </c>
       <c r="M16" s="2">
@@ -2832,10 +2837,10 @@
       <c r="H17" s="4">
         <v>0.95334335702528461</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="9">
         <v>0.27196687116124607</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="9">
         <v>0.32136824878237358</v>
       </c>
       <c r="M17" s="2">
@@ -3699,7 +3704,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A18:F34">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3710,6 +3715,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>